<commit_message>
wokring stesp 2 before 3.
</commit_message>
<xml_diff>
--- a/output/invoice_records.xlsx
+++ b/output/invoice_records.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2263"/>
+  <dimension ref="A1:E2430"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38411,12 +38411,2850 @@
           <t>s1</t>
         </is>
       </c>
-      <c r="B2263" t="inlineStr"/>
-      <c r="C2263" t="inlineStr"/>
-      <c r="D2263" t="inlineStr"/>
       <c r="E2263" t="inlineStr">
         <is>
           <t>2025-09-06 20:26:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="2264">
+      <c r="A2264" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2264" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2264" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:32:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="2265">
+      <c r="A2265" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2265" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2265" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2266">
+      <c r="A2266" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2266" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2266" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2267">
+      <c r="A2267" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2267" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2267" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2268">
+      <c r="A2268" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2268" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2268" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2269">
+      <c r="A2269" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2269" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2269" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2270">
+      <c r="A2270" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2270" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2270" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="2271">
+      <c r="A2271" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2271" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2271" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="2272">
+      <c r="A2272" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2272" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2272" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="2273">
+      <c r="A2273" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2273" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2273" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="2274">
+      <c r="A2274" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2274" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2274" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="2275">
+      <c r="A2275" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2275" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2275" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2276">
+      <c r="A2276" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2276" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2276" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2277">
+      <c r="A2277" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2277" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2277" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2278">
+      <c r="A2278" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2278" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2278" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2279">
+      <c r="A2279" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2279" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2279" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2280">
+      <c r="A2280" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2280" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2280" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2281">
+      <c r="A2281" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2281" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2281" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="2282">
+      <c r="A2282" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2282" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2282" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="2283">
+      <c r="A2283" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2283" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2283" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="2284">
+      <c r="A2284" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2284" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2284" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="2285">
+      <c r="A2285" t="inlineStr">
+        <is>
+          <t>skewed</t>
+        </is>
+      </c>
+      <c r="B2285" t="inlineStr">
+        <is>
+          <t>8513</t>
+        </is>
+      </c>
+      <c r="E2285" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:33:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="2286">
+      <c r="A2286" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2286" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2286" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="2287">
+      <c r="A2287" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2287" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2287" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="2288">
+      <c r="A2288" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2288" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2288" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="2289">
+      <c r="A2289" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2289" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2289" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="2290">
+      <c r="A2290" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2290" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2290" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="2291">
+      <c r="A2291" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2291" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2291" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2292">
+      <c r="A2292" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2292" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2292" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2293">
+      <c r="A2293" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2293" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2293" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="2294">
+      <c r="A2294" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2294" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2294" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="2295">
+      <c r="A2295" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2295" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2295" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="2296">
+      <c r="A2296" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2296" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2296" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="2297">
+      <c r="A2297" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2297" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2297" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="2298">
+      <c r="A2298" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2298" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2298" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="2299">
+      <c r="A2299" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2299" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2299" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="2300">
+      <c r="A2300" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2300" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2300" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:34:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="2301">
+      <c r="A2301" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2301" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2301" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="2302">
+      <c r="A2302" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2302" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2302" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="2303">
+      <c r="A2303" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2303" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2303" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="2304">
+      <c r="A2304" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2304" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2304" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="2305">
+      <c r="A2305" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2305" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2305" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="2306">
+      <c r="A2306" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2306" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2306" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="2307">
+      <c r="A2307" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2307" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2307" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="2308">
+      <c r="A2308" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2308" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2308" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="2309">
+      <c r="A2309" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2309" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2309" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="2310">
+      <c r="A2310" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2310" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2310" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="2311">
+      <c r="A2311" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2311" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2311" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="2312">
+      <c r="A2312" t="inlineStr">
+        <is>
+          <t>skewed</t>
+        </is>
+      </c>
+      <c r="B2312" t="inlineStr">
+        <is>
+          <t>Ocvzuu 8513</t>
+        </is>
+      </c>
+      <c r="E2312" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:35:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2313">
+      <c r="A2313" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2313" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2313" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="2314">
+      <c r="A2314" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2314" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2314" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="2315">
+      <c r="A2315" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2315" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2315" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="2316">
+      <c r="A2316" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2316" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2316" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="2317">
+      <c r="A2317" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2317" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2317" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="2318">
+      <c r="A2318" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2318" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2318" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="2319">
+      <c r="A2319" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2319" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2319" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="2320">
+      <c r="A2320" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2320" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2320" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="2321">
+      <c r="A2321" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2321" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2321" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="2322">
+      <c r="A2322" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2322" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2322" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="2323">
+      <c r="A2323" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2323" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2323" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="2324">
+      <c r="A2324" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2324" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2324" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2325">
+      <c r="A2325" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2325" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2325" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2326">
+      <c r="A2326" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2326" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2326" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2327">
+      <c r="A2327" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2327" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2327" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2328">
+      <c r="A2328" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2328" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2328" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="2329">
+      <c r="A2329" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2329" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2329" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2330">
+      <c r="A2330" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2330" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2330" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2331">
+      <c r="A2331" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2331" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2331" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="2332">
+      <c r="A2332" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2332" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2332" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="2333">
+      <c r="A2333" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2333" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2333" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="2334">
+      <c r="A2334" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2334" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2334" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="2335">
+      <c r="A2335" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2335" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2335" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:36:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2336">
+      <c r="A2336" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2336" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2336" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="2337">
+      <c r="A2337" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2337" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2337" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="2338">
+      <c r="A2338" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2338" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2338" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2339">
+      <c r="A2339" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2339" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2339" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2340">
+      <c r="A2340" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2340" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2340" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2341">
+      <c r="A2341" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2341" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2341" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2342">
+      <c r="A2342" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2342" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2342" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2343">
+      <c r="A2343" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2343" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2343" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2344">
+      <c r="A2344" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2344" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2344" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2345">
+      <c r="A2345" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2345" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2345" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2346">
+      <c r="A2346" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2346" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2346" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2347">
+      <c r="A2347" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2347" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2347" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2348">
+      <c r="A2348" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2348" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2348" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2349">
+      <c r="A2349" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2349" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2349" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2350">
+      <c r="A2350" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2350" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2350" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2351">
+      <c r="A2351" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2351" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2351" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2352">
+      <c r="A2352" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2352" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2352" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2353">
+      <c r="A2353" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2353" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2353" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2354">
+      <c r="A2354" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2354" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2354" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2355">
+      <c r="A2355" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2355" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2355" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2356">
+      <c r="A2356" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2356" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2356" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="2357">
+      <c r="A2357" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2357" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2357" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="2358">
+      <c r="A2358" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2358" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2358" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:39:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="2359">
+      <c r="A2359" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2359" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2359" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2360">
+      <c r="A2360" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2360" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2360" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2361">
+      <c r="A2361" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2361" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2361" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2362">
+      <c r="A2362" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2362" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2362" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2363">
+      <c r="A2363" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2363" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2363" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2364">
+      <c r="A2364" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2364" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2364" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2365">
+      <c r="A2365" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2365" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2365" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2366">
+      <c r="A2366" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2366" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2366" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2367">
+      <c r="A2367" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2367" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2367" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2368">
+      <c r="A2368" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2368" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2368" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2369">
+      <c r="A2369" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2369" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2369" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2370">
+      <c r="A2370" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2370" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2370" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2371">
+      <c r="A2371" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2371" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2371" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2372">
+      <c r="A2372" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2372" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2372" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2373">
+      <c r="A2373" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2373" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2373" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="2374">
+      <c r="A2374" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2374" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2374" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="2375">
+      <c r="A2375" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2375" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2375" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="2376">
+      <c r="A2376" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2376" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2376" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="2377">
+      <c r="A2377" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2377" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2377" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="2378">
+      <c r="A2378" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2378" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2378" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="2379">
+      <c r="A2379" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2379" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2379" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="2380">
+      <c r="A2380" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2380" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2380" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="2381">
+      <c r="A2381" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2381" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2381" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:40:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="2382">
+      <c r="A2382" t="inlineStr">
+        <is>
+          <t>skwed</t>
+        </is>
+      </c>
+      <c r="B2382" t="inlineStr">
+        <is>
+          <t>8513</t>
+        </is>
+      </c>
+      <c r="E2382" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="2383">
+      <c r="A2383" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2383" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2383" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="2384">
+      <c r="A2384" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2384" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2384" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="2385">
+      <c r="A2385" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2385" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2385" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="2386">
+      <c r="A2386" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2386" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2386" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="2387">
+      <c r="A2387" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2387" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2387" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2388">
+      <c r="A2388" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2388" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2388" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2389">
+      <c r="A2389" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2389" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2389" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2390">
+      <c r="A2390" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2390" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2390" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2391">
+      <c r="A2391" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2391" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2391" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2392">
+      <c r="A2392" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2392" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2392" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2393">
+      <c r="A2393" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2393" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2393" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2394">
+      <c r="A2394" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2394" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2394" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2395">
+      <c r="A2395" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2395" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2395" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="2396">
+      <c r="A2396" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2396" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2396" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="2397">
+      <c r="A2397" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2397" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2397" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="2398">
+      <c r="A2398" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2398" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2398" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="2399">
+      <c r="A2399" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2399" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2399" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2400">
+      <c r="A2400" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2400" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2400" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2401">
+      <c r="A2401" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2401" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2401" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2402">
+      <c r="A2402" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2402" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2402" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2403">
+      <c r="A2403" t="inlineStr">
+        <is>
+          <t>skwed</t>
+        </is>
+      </c>
+      <c r="B2403" t="inlineStr">
+        <is>
+          <t>8513</t>
+        </is>
+      </c>
+      <c r="E2403" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2404">
+      <c r="A2404" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2404" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2404" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="2405">
+      <c r="A2405" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2405" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2405" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="2406">
+      <c r="A2406" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2406" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2406" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:41:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="2407">
+      <c r="A2407" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2407" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2407" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="2408">
+      <c r="A2408" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2408" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2408" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="2409">
+      <c r="A2409" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2409" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2409" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="2410">
+      <c r="A2410" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2410" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2410" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="2411">
+      <c r="A2411" t="inlineStr">
+        <is>
+          <t>ssdf21</t>
+        </is>
+      </c>
+      <c r="B2411" t="inlineStr">
+        <is>
+          <t>#1024</t>
+        </is>
+      </c>
+      <c r="E2411" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="2412">
+      <c r="A2412" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2412" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2412" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="2413">
+      <c r="A2413" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2413" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2413" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2414">
+      <c r="A2414" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2414" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2414" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2415">
+      <c r="A2415" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2415" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2415" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2416">
+      <c r="A2416" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2416" t="inlineStr">
+        <is>
+          <t>Blll T0:</t>
+        </is>
+      </c>
+      <c r="E2416" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2417">
+      <c r="A2417" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2417" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2417" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2418">
+      <c r="A2418" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2418" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2418" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2419">
+      <c r="A2419" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2419" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2419" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="2420">
+      <c r="A2420" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2420" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2420" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2421">
+      <c r="A2421" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="B2421" t="inlineStr">
+        <is>
+          <t>Invoice No. 12345</t>
+        </is>
+      </c>
+      <c r="E2421" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="2422">
+      <c r="A2422" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2422" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2422" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2423">
+      <c r="A2423" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2423" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2423" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="2424">
+      <c r="A2424" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2424" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2424" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2425">
+      <c r="A2425" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2425" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2425" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="2426">
+      <c r="A2426" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2426" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2426" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2427">
+      <c r="A2427" t="inlineStr">
+        <is>
+          <t>skwed</t>
+        </is>
+      </c>
+      <c r="B2427" t="inlineStr">
+        <is>
+          <t>8513</t>
+        </is>
+      </c>
+      <c r="E2427" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="2428">
+      <c r="A2428" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2428" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="E2428" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="2429">
+      <c r="A2429" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2429" t="inlineStr">
+        <is>
+          <t>55888800000998700</t>
+        </is>
+      </c>
+      <c r="E2429" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="2430">
+      <c r="A2430" t="inlineStr">
+        <is>
+          <t>superstore1</t>
+        </is>
+      </c>
+      <c r="B2430" t="inlineStr">
+        <is>
+          <t>#40954</t>
+        </is>
+      </c>
+      <c r="C2430" t="inlineStr"/>
+      <c r="D2430" t="inlineStr"/>
+      <c r="E2430" t="inlineStr">
+        <is>
+          <t>2025-09-06 20:42:43</t>
         </is>
       </c>
     </row>

</xml_diff>